<commit_message>
adding selenium bot for tribal wars
</commit_message>
<xml_diff>
--- a/IMDB Movie Ratings.xlsx
+++ b/IMDB Movie Ratings.xlsx
@@ -3993,12 +3993,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>The Seventh Seal</t>
+          <t>The Elephant Man</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>(1957)</t>
+          <t>(1980)</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
@@ -4015,12 +4015,12 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>The Elephant Man</t>
+          <t>The Seventh Seal</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>(1980)</t>
+          <t>(1957)</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -5863,12 +5863,12 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Hera Pheri</t>
+          <t>96</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>(2000)</t>
+          <t>(2018)</t>
         </is>
       </c>
       <c r="D248" t="inlineStr">
@@ -5885,12 +5885,12 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>Fanny and Alexander</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>(2018)</t>
+          <t>(1982)</t>
         </is>
       </c>
       <c r="D249" t="inlineStr">
@@ -5907,12 +5907,12 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Fanny and Alexander</t>
+          <t>Hera Pheri</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>(1982)</t>
+          <t>(2000)</t>
         </is>
       </c>
       <c r="D250" t="inlineStr">
@@ -5929,12 +5929,12 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>The Battle of Algiers</t>
+          <t>Soorarai Pottru</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>(1966)</t>
+          <t>(2020)</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">

</xml_diff>

<commit_message>
adding tribal wars bot files
</commit_message>
<xml_diff>
--- a/IMDB Movie Ratings.xlsx
+++ b/IMDB Movie Ratings.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>9.1</t>
+          <t>9.2</t>
         </is>
       </c>
     </row>
@@ -495,12 +495,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>The Godfather: Part II</t>
+          <t>The Dark Knight</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(1974)</t>
+          <t>(2008)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -517,12 +517,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>The Dark Knight</t>
+          <t>The Godfather: Part II</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>(2008)</t>
+          <t>(1974)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -549,7 +549,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>8.9</t>
+          <t>9.0</t>
         </is>
       </c>
     </row>
@@ -615,7 +615,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>8.8</t>
+          <t>8.9</t>
         </is>
       </c>
     </row>
@@ -627,12 +627,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>The Good, the Bad and the Ugly</t>
+          <t>The Lord of the Rings: The Fellowship of the Ring</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>(1966)</t>
+          <t>(2001)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -649,12 +649,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>The Lord of the Rings: The Fellowship of the Ring</t>
+          <t>The Good, the Bad and the Ugly</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>(2001)</t>
+          <t>(1966)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -671,17 +671,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Fight Club</t>
+          <t>Forrest Gump</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>(1999)</t>
+          <t>(1994)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>8.7</t>
+          <t>8.8</t>
         </is>
       </c>
     </row>
@@ -693,17 +693,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Forrest Gump</t>
+          <t>Fight Club</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>(1994)</t>
+          <t>(1999)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>8.7</t>
+          <t>8.8</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>8.6</t>
+          <t>8.7</t>
         </is>
       </c>
     </row>
@@ -847,12 +847,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Seven Samurai</t>
+          <t>Se7en</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>(1954)</t>
+          <t>(1995)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -869,12 +869,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Se7en</t>
+          <t>Seven Samurai</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>(1995)</t>
+          <t>(1954)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -891,12 +891,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>The Silence of the Lambs</t>
+          <t>It's a Wonderful Life</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>(1991)</t>
+          <t>(1946)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -913,12 +913,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>City of God</t>
+          <t>The Silence of the Lambs</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>(2002)</t>
+          <t>(1991)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -935,12 +935,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Life Is Beautiful</t>
+          <t>Saving Private Ryan</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>(1997)</t>
+          <t>(1998)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -957,12 +957,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>It's a Wonderful Life</t>
+          <t>City of God</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>(1946)</t>
+          <t>(2002)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -979,12 +979,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Saving Private Ryan</t>
+          <t>Life Is Beautiful</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>(1998)</t>
+          <t>(1997)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1001,17 +1001,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Star Wars</t>
+          <t>The Green Mile</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>(1977)</t>
+          <t>(1999)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>8.5</t>
+          <t>8.6</t>
         </is>
       </c>
     </row>
@@ -1023,17 +1023,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Interstellar</t>
+          <t>Star Wars</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>(2014)</t>
+          <t>(1977)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>8.5</t>
+          <t>8.6</t>
         </is>
       </c>
     </row>
@@ -1045,17 +1045,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Spirited Away</t>
+          <t>Interstellar</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>(2001)</t>
+          <t>(2014)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>8.5</t>
+          <t>8.6</t>
         </is>
       </c>
     </row>
@@ -1067,12 +1067,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>The Green Mile</t>
+          <t>Terminator 2: Judgment Day</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>(1999)</t>
+          <t>(1991)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1089,12 +1089,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Parasite</t>
+          <t>Back to the Future</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>(2019)</t>
+          <t>(1985)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1111,12 +1111,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Spider-Man: No Way Home</t>
+          <t>Spirited Away</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>(2021)</t>
+          <t>(2001)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1133,12 +1133,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Léon: The Professional</t>
+          <t>Psycho</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>(1994)</t>
+          <t>(1960)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1155,12 +1155,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Hara-Kiri</t>
+          <t>Léon: The Professional</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>(1962)</t>
+          <t>(1994)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1199,12 +1199,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Terminator 2: Judgment Day</t>
+          <t>Parasite</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>(1991)</t>
+          <t>(2019)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1221,12 +1221,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Back to the Future</t>
+          <t>The Lion King</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>(1985)</t>
+          <t>(1994)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1243,12 +1243,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>The Lion King</t>
+          <t>Gladiator</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>(1994)</t>
+          <t>(2000)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1265,12 +1265,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Psycho</t>
+          <t>American History X</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>(1960)</t>
+          <t>(1998)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1309,12 +1309,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Modern Times</t>
+          <t>Spider-Man: No Way Home</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>(1936)</t>
+          <t>(2021)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1331,12 +1331,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Grave of the Fireflies</t>
+          <t>The Departed</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>(1988)</t>
+          <t>(2006)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1353,12 +1353,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>American History X</t>
+          <t>The Prestige</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>(1998)</t>
+          <t>(2006)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1375,12 +1375,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Whiplash</t>
+          <t>Casablanca</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>(2014)</t>
+          <t>(1942)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1397,12 +1397,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Gladiator</t>
+          <t>Whiplash</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>(2000)</t>
+          <t>(2014)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1419,12 +1419,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>The Departed</t>
+          <t>The Intouchables</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>(2006)</t>
+          <t>(2011)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1441,12 +1441,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>City Lights</t>
+          <t>Modern Times</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>(1931)</t>
+          <t>(1936)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1463,12 +1463,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>The Intouchables</t>
+          <t>Once Upon a Time in the West</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>(2011)</t>
+          <t>(1968)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1485,12 +1485,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>The Prestige</t>
+          <t>Hara-Kiri</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>(2006)</t>
+          <t>(1962)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1507,17 +1507,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Casablanca</t>
+          <t>Grave of the Fireflies</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>(1942)</t>
+          <t>(1988)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>8.4</t>
+          <t>8.5</t>
         </is>
       </c>
     </row>
@@ -1529,12 +1529,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Once Upon a Time in the West</t>
+          <t>Alien</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>(1968)</t>
+          <t>(1979)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1573,12 +1573,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Cinema Paradiso</t>
+          <t>City Lights</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>(1988)</t>
+          <t>(1931)</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1595,12 +1595,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Alien</t>
+          <t>Memento</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>(1979)</t>
+          <t>(2000)</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1639,12 +1639,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Memento</t>
+          <t>Cinema Paradiso</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>(2000)</t>
+          <t>(1988)</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1683,12 +1683,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>The Great Dictator</t>
+          <t>Django Unchained</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>(1940)</t>
+          <t>(2012)</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1705,12 +1705,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Django Unchained</t>
+          <t>WALL·E</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>(2012)</t>
+          <t>(2008)</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1749,12 +1749,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Paths of Glory</t>
+          <t>Sunset Blvd.</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>(1957)</t>
+          <t>(1950)</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1771,12 +1771,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Sunset Blvd.</t>
+          <t>The Shining</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>(1950)</t>
+          <t>(1980)</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1793,12 +1793,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>WALL·E</t>
+          <t>Paths of Glory</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>(2008)</t>
+          <t>(1957)</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1815,12 +1815,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Avengers: Infinity War</t>
+          <t>The Great Dictator</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>(2018)</t>
+          <t>(1940)</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Spider-Man: Into the Spider-Verse</t>
+          <t>Avengers: Infinity War</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1881,12 +1881,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>The Shining</t>
+          <t>The Batman</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>(1980)</t>
+          <t>(2022)</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -1903,12 +1903,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Dr. Strangelove or: How I Learned to Stop Worrying and Love the Bomb</t>
+          <t>Aliens</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>(1964)</t>
+          <t>(1986)</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -1925,12 +1925,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Princess Mononoke</t>
+          <t>American Beauty</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>(1997)</t>
+          <t>(1999)</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -1947,12 +1947,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Old Boy</t>
+          <t>The Dark Knight Rises</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>(2003)</t>
+          <t>(2012)</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -1969,12 +1969,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Joker</t>
+          <t>Dr. Strangelove or: How I Learned to Stop Worrying and Love the Bomb</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>(2019)</t>
+          <t>(1964)</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -1991,12 +1991,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Your Name.</t>
+          <t>Joker</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>(2016)</t>
+          <t>(2019)</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2013,12 +2013,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Coco</t>
+          <t>Spider-Man: Into the Spider-Verse</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>(2017)</t>
+          <t>(2018)</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2035,12 +2035,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>The Dark Knight Rises</t>
+          <t>Old Boy</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>(2012)</t>
+          <t>(2003)</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2057,12 +2057,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Aliens</t>
+          <t>Braveheart</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>(1986)</t>
+          <t>(1995)</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2079,12 +2079,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Once Upon a Time in America</t>
+          <t>Toy Story</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>(1984)</t>
+          <t>(1995)</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2101,12 +2101,12 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Avengers: Endgame</t>
+          <t>Amadeus</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>(2019)</t>
+          <t>(1984)</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2123,12 +2123,12 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Capernaum</t>
+          <t>Coco</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>(2018)</t>
+          <t>(2017)</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2145,12 +2145,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>The Boat</t>
+          <t>Inglourious Basterds</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>(1981)</t>
+          <t>(2009)</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2167,12 +2167,12 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>High and Low</t>
+          <t>The Boat</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>(1963)</t>
+          <t>(1981)</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2189,12 +2189,12 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>3 Idiots</t>
+          <t>Avengers: Endgame</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>(2009)</t>
+          <t>(2019)</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2211,12 +2211,12 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Toy Story</t>
+          <t>Princess Mononoke</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>(1995)</t>
+          <t>(1997)</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Amadeus</t>
+          <t>Once Upon a Time in America</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2255,12 +2255,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>American Beauty</t>
+          <t>Good Will Hunting</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>(1999)</t>
+          <t>(1997)</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2277,12 +2277,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Braveheart</t>
+          <t>Toy Story 3</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>(1995)</t>
+          <t>(2010)</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2299,12 +2299,12 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Inglourious Basterds</t>
+          <t>Requiem for a Dream</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>(2009)</t>
+          <t>(2000)</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2321,12 +2321,12 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Good Will Hunting</t>
+          <t>3 Idiots</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>(1997)</t>
+          <t>(2009)</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2343,12 +2343,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Hamilton</t>
+          <t>Singin' in the Rain</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>(2020)</t>
+          <t>(1952)</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2365,12 +2365,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Come and See</t>
+          <t>Your Name.</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>(1985)</t>
+          <t>(2016)</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2409,12 +2409,12 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>2001: A Space Odyssey</t>
+          <t>Reservoir Dogs</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>(1968)</t>
+          <t>(1992)</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2431,12 +2431,12 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Reservoir Dogs</t>
+          <t>Eternal Sunshine of the Spotless Mind</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>(1992)</t>
+          <t>(2004)</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2453,12 +2453,12 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Like Stars on Earth</t>
+          <t>2001: A Space Odyssey</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>(2007)</t>
+          <t>(1968)</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2475,12 +2475,12 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Vertigo</t>
+          <t>Citizen Kane</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>(1958)</t>
+          <t>(1941)</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2497,12 +2497,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>High and Low</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>(1931)</t>
+          <t>(1963)</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2519,12 +2519,12 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>The Hunt</t>
+          <t>Lawrence of Arabia</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>(2012)</t>
+          <t>(1962)</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2541,12 +2541,12 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Citizen Kane</t>
+          <t>M</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>(1941)</t>
+          <t>(1931)</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2563,12 +2563,12 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Singin' in the Rain</t>
+          <t>Capernaum</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>(1952)</t>
+          <t>(2018)</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -2585,12 +2585,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Requiem for a Dream</t>
+          <t>North by Northwest</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>(2000)</t>
+          <t>(1959)</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -2607,12 +2607,12 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>North by Northwest</t>
+          <t>The Hunt</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>(1959)</t>
+          <t>(2012)</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -2629,12 +2629,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Ikiru</t>
+          <t>Vertigo</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>(1952)</t>
+          <t>(1958)</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -2651,12 +2651,12 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Eternal Sunshine of the Spotless Mind</t>
+          <t>Amélie</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>(2004)</t>
+          <t>(2001)</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -2673,12 +2673,12 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Bicycle Thieves</t>
+          <t>A Clockwork Orange</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>(1948)</t>
+          <t>(1971)</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -2695,12 +2695,12 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Lawrence of Arabia</t>
+          <t>Full Metal Jacket</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>(1962)</t>
+          <t>(1987)</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -2717,12 +2717,12 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>The Kid</t>
+          <t>Scarface</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>(1921)</t>
+          <t>(1983)</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -2739,12 +2739,12 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Incendies</t>
+          <t>Double Indemnity</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>(2010)</t>
+          <t>(1944)</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -2761,12 +2761,12 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Full Metal Jacket</t>
+          <t>Come and See</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>(1987)</t>
+          <t>(1985)</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -2783,12 +2783,12 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Dangal</t>
+          <t>The Apartment</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>(2016)</t>
+          <t>(1960)</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -2805,12 +2805,12 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>The Apartment</t>
+          <t>Taxi Driver</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>(1960)</t>
+          <t>(1976)</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -2827,12 +2827,12 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Double Indemnity</t>
+          <t>Hamilton</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>(1944)</t>
+          <t>(2020)</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -2849,12 +2849,12 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Metropolis</t>
+          <t>To Kill a Mockingbird</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>(1927)</t>
+          <t>(1962)</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -2871,12 +2871,12 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>A Clockwork Orange</t>
+          <t>L.A. Confidential</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>(1971)</t>
+          <t>(1997)</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -2893,12 +2893,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Taxi Driver</t>
+          <t>The Sting</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>(1976)</t>
+          <t>(1973)</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -2915,12 +2915,12 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>The Father</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>(2020)</t>
+          <t>(2009)</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -2937,12 +2937,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>A Separation</t>
+          <t>Heat</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>(2011)</t>
+          <t>(1995)</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -2959,12 +2959,12 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>The Sting</t>
+          <t>Snatch</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>(1973)</t>
+          <t>(2000)</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -2981,12 +2981,12 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Scarface</t>
+          <t>Ikiru</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>(1983)</t>
+          <t>(1952)</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3003,12 +3003,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Snatch</t>
+          <t>Die Hard</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>(2000)</t>
+          <t>(1988)</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3025,12 +3025,12 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>1917</t>
+          <t>Indiana Jones and the Last Crusade</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>(2019)</t>
+          <t>(1989)</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3047,12 +3047,12 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Amélie</t>
+          <t>A Separation</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>(2001)</t>
+          <t>(2011)</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3069,12 +3069,12 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>To Kill a Mockingbird</t>
+          <t>Metropolis</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>(1962)</t>
+          <t>(1927)</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3091,12 +3091,12 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Toy Story 3</t>
+          <t>Bicycle Thieves</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>(2010)</t>
+          <t>(1948)</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3113,12 +3113,12 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>For a Few Dollars More</t>
+          <t>Incendies</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>(1965)</t>
+          <t>(2010)</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3135,12 +3135,12 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>1917</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>(2009)</t>
+          <t>(2019)</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3157,12 +3157,12 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Indiana Jones and the Last Crusade</t>
+          <t>Like Stars on Earth</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>(1989)</t>
+          <t>(2007)</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3179,12 +3179,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Pather Panchali</t>
+          <t>Batman Begins</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>(1955)</t>
+          <t>(2005)</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3201,12 +3201,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Heat</t>
+          <t>For a Few Dollars More</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>(1995)</t>
+          <t>(1965)</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -3223,12 +3223,12 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>L.A. Confidential</t>
+          <t>Dangal</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>(1997)</t>
+          <t>(2016)</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -3245,12 +3245,12 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Ran</t>
+          <t>Downfall</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>(1985)</t>
+          <t>(2004)</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -3267,12 +3267,12 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Die Hard</t>
+          <t>The Kid</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>(1988)</t>
+          <t>(1921)</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -3289,12 +3289,12 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Yojimbo</t>
+          <t>Some Like It Hot</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>(1961)</t>
+          <t>(1959)</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3311,12 +3311,12 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Green Book</t>
+          <t>The Father</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>(2018)</t>
+          <t>(2020)</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -3333,12 +3333,12 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Downfall</t>
+          <t>All About Eve</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>(2004)</t>
+          <t>(1950)</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -3355,12 +3355,12 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Rashomon</t>
+          <t>Green Book</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>(1950)</t>
+          <t>(2018)</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -3377,12 +3377,12 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>All About Eve</t>
+          <t>The Wolf of Wall Street</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>(1950)</t>
+          <t>(2013)</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -3399,12 +3399,12 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Monty Python and the Holy Grail</t>
+          <t>Unforgiven</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>(1975)</t>
+          <t>(1992)</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -3421,12 +3421,12 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Some Like It Hot</t>
+          <t>Casino</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>(1959)</t>
+          <t>(1995)</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -3443,12 +3443,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Batman Begins</t>
+          <t>Pan's Labyrinth</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>(2005)</t>
+          <t>(2006)</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -3465,12 +3465,12 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Unforgiven</t>
+          <t>Judgment at Nuremberg</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>(1992)</t>
+          <t>(1961)</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -3487,12 +3487,12 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Children of Heaven</t>
+          <t>Ran</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>(1997)</t>
+          <t>(1985)</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -3509,12 +3509,12 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Jai Bhim</t>
+          <t>A Beautiful Mind</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>(2021)</t>
+          <t>(2001)</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -3531,12 +3531,12 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>The Wolf of Wall Street</t>
+          <t>The Sixth Sense</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>(2013)</t>
+          <t>(1999)</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -3553,12 +3553,12 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Howl's Moving Castle</t>
+          <t>Monty Python and the Holy Grail</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>(2004)</t>
+          <t>(1975)</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -3575,12 +3575,12 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Judgment at Nuremberg</t>
+          <t>There Will Be Blood</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>(1961)</t>
+          <t>(2007)</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -3597,12 +3597,12 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>There Will Be Blood</t>
+          <t>The Truman Show</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>(2007)</t>
+          <t>(1998)</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -3619,12 +3619,12 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Casino</t>
+          <t>Yojimbo</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>(1995)</t>
+          <t>(1961)</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -3641,12 +3641,12 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>The Great Escape</t>
+          <t>The Treasure of the Sierra Madre</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>(1963)</t>
+          <t>(1948)</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -3663,12 +3663,12 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>The Treasure of the Sierra Madre</t>
+          <t>Shutter Island</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>(1948)</t>
+          <t>(2010)</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -3685,17 +3685,17 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Pan's Labyrinth</t>
+          <t>The Great Escape</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>(2006)</t>
+          <t>(1963)</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>8.2</t>
         </is>
       </c>
     </row>
@@ -3707,12 +3707,12 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>A Beautiful Mind</t>
+          <t>Rashomon</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>(2001)</t>
+          <t>(1950)</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -3729,12 +3729,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>The Secret in Their Eyes</t>
+          <t>Jurassic Park</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>(2009)</t>
+          <t>(1993)</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -3751,12 +3751,12 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Raging Bull</t>
+          <t>Kill Bill: Vol. 1</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>(1980)</t>
+          <t>(2003)</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -3773,12 +3773,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Chinatown</t>
+          <t>Finding Nemo</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>(1974)</t>
+          <t>(2003)</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -3795,12 +3795,12 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Shutter Island</t>
+          <t>No Country for Old Men</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>(2010)</t>
+          <t>(2007)</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -3817,12 +3817,12 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>My Neighbor Totoro</t>
+          <t>Raging Bull</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>(1988)</t>
+          <t>(1980)</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -3839,12 +3839,12 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Lock, Stock and Two Smoking Barrels</t>
+          <t>The Elephant Man</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>(1998)</t>
+          <t>(1980)</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -3861,12 +3861,12 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>No Country for Old Men</t>
+          <t>V for Vendetta</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>(2007)</t>
+          <t>(2005)</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -3883,12 +3883,12 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Klaus</t>
+          <t>Gone with the Wind</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>(2019)</t>
+          <t>(1939)</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -3905,12 +3905,12 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>The Thing</t>
+          <t>Chinatown</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>(1982)</t>
+          <t>(1974)</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -3927,12 +3927,12 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Dial M for Murder</t>
+          <t>Inside Out</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>(1954)</t>
+          <t>(2015)</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -3949,12 +3949,12 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>The Gold Rush</t>
+          <t>Lock, Stock and Two Smoking Barrels</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>(1925)</t>
+          <t>(1998)</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -3971,12 +3971,12 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Three Billboards Outside Ebbing, Missouri</t>
+          <t>The Thing</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>(2017)</t>
+          <t>(1982)</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -3993,12 +3993,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>The Elephant Man</t>
+          <t>Dial M for Murder</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>(1980)</t>
+          <t>(1954)</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
@@ -4015,12 +4015,12 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>The Seventh Seal</t>
+          <t>The Secret in Their Eyes</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>(1957)</t>
+          <t>(2009)</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -4037,12 +4037,12 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>The Sixth Sense</t>
+          <t>Howl's Moving Castle</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>(1999)</t>
+          <t>(2004)</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
@@ -4059,12 +4059,12 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Jurassic Park</t>
+          <t>The Bridge on the River Kwai</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>(1993)</t>
+          <t>(1957)</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
@@ -4081,12 +4081,12 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>The Truman Show</t>
+          <t>Trainspotting</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>(1998)</t>
+          <t>(1996)</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
@@ -4103,12 +4103,12 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Dersu Uzala</t>
+          <t>Three Billboards Outside Ebbing, Missouri</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>(1975)</t>
+          <t>(2017)</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -4125,12 +4125,12 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Wild Strawberries</t>
+          <t>Warrior</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>(1957)</t>
+          <t>(2011)</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
@@ -4147,12 +4147,12 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>The Third Man</t>
+          <t>Gran Torino</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>(1949)</t>
+          <t>(2008)</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
@@ -4169,12 +4169,12 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Memories of Murder</t>
+          <t>Fargo</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>(2003)</t>
+          <t>(1996)</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
@@ -4191,12 +4191,12 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>V for Vendetta</t>
+          <t>My Neighbor Totoro</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>(2005)</t>
+          <t>(1988)</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -4213,12 +4213,12 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Blade Runner</t>
+          <t>Prisoners</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>(1982)</t>
+          <t>(2013)</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -4235,12 +4235,12 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Trainspotting</t>
+          <t>Million Dollar Baby</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>(1996)</t>
+          <t>(2004)</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
@@ -4257,12 +4257,12 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Fargo</t>
+          <t>Blade Runner</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>(1996)</t>
+          <t>(1982)</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
@@ -4279,12 +4279,12 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>The Bridge on the River Kwai</t>
+          <t>The Gold Rush</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>(1957)</t>
+          <t>(1925)</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
@@ -4301,12 +4301,12 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Inside Out</t>
+          <t>Catch Me If You Can</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>(2015)</t>
+          <t>(2002)</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
@@ -4323,12 +4323,12 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Kill Bill: Vol. 1</t>
+          <t>On the Waterfront</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>(2003)</t>
+          <t>(1954)</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
@@ -4345,12 +4345,12 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Finding Nemo</t>
+          <t>Children of Heaven</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>(2003)</t>
+          <t>(1997)</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
@@ -4367,12 +4367,12 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Warrior</t>
+          <t>The Third Man</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>(2011)</t>
+          <t>(1949)</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -4389,12 +4389,12 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Gone with the Wind</t>
+          <t>Harry Potter and the Deathly Hallows: Part 2</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>(1939)</t>
+          <t>(2011)</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
@@ -4411,12 +4411,12 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Tokyo Story</t>
+          <t>Gone Girl</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>(1953)</t>
+          <t>(2014)</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
@@ -4433,12 +4433,12 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>On the Waterfront</t>
+          <t>Ben-Hur</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>(1954)</t>
+          <t>(1959)</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
@@ -4455,12 +4455,12 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>My Father and My Son</t>
+          <t>12 Years a Slave</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>(2005)</t>
+          <t>(2013)</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
@@ -4477,12 +4477,12 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Prisoners</t>
+          <t>The General</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>(2013)</t>
+          <t>(1926)</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
@@ -4499,12 +4499,12 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Wild Tales</t>
+          <t>The Deer Hunter</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>(2014)</t>
+          <t>(1978)</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
@@ -4521,12 +4521,12 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>The Grand Budapest Hotel</t>
+          <t>Wild Strawberries</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>(2014)</t>
+          <t>(1957)</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
@@ -4543,12 +4543,12 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Stalker</t>
+          <t>Pather Panchali</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>(1979)</t>
+          <t>(1955)</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
@@ -4565,12 +4565,12 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>The Deer Hunter</t>
+          <t>Before Sunrise</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>(1978)</t>
+          <t>(1995)</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
@@ -4587,12 +4587,12 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Gran Torino</t>
+          <t>In the Name of the Father</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>(2008)</t>
+          <t>(1993)</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
@@ -4609,12 +4609,12 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Sherlock Jr.</t>
+          <t>Mr. Smith Goes to Washington</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>(1924)</t>
+          <t>(1939)</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -4631,12 +4631,12 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>The General</t>
+          <t>The Grand Budapest Hotel</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>(1926)</t>
+          <t>(2014)</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
@@ -4653,12 +4653,12 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Persona</t>
+          <t>Room</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>(1966)</t>
+          <t>(2015)</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
@@ -4675,12 +4675,12 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Before Sunrise</t>
+          <t>Sherlock Jr.</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>(1995)</t>
+          <t>(1924)</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
@@ -4697,12 +4697,12 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Catch Me If You Can</t>
+          <t>Hacksaw Ridge</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>(2002)</t>
+          <t>(2016)</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
@@ -4719,12 +4719,12 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Mary and Max</t>
+          <t>How to Train Your Dragon</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>(2009)</t>
+          <t>(2010)</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
@@ -4741,12 +4741,12 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Barry Lyndon</t>
+          <t>The Wages of Fear</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>(1975)</t>
+          <t>(1953)</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
@@ -4763,12 +4763,12 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Mr. Smith Goes to Washington</t>
+          <t>Memories of Murder</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>(1939)</t>
+          <t>(2003)</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
@@ -4785,12 +4785,12 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>In the Name of the Father</t>
+          <t>The Seventh Seal</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>(1993)</t>
+          <t>(1957)</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
@@ -4807,12 +4807,12 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Hacksaw Ridge</t>
+          <t>Barry Lyndon</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>(2016)</t>
+          <t>(1975)</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
@@ -4829,12 +4829,12 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Gone Girl</t>
+          <t>The Big Lebowski</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>(2014)</t>
+          <t>(1998)</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
@@ -4851,7 +4851,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Room</t>
+          <t>Mad Max: Fury Road</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
@@ -4873,12 +4873,12 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Z</t>
+          <t>Klaus</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>(1969)</t>
+          <t>(2019)</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
@@ -4895,12 +4895,12 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Andhadhun</t>
+          <t>Wild Tales</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>(2018)</t>
+          <t>(2014)</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
@@ -4917,12 +4917,12 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Ford v Ferrari</t>
+          <t>Monsters, Inc.</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>(2019)</t>
+          <t>(2001)</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
@@ -4939,12 +4939,12 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>The Passion of Joan of Arc</t>
+          <t>Mary and Max</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>(1928)</t>
+          <t>(2009)</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
@@ -4961,12 +4961,12 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>12 Years a Slave</t>
+          <t>Jaws</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>(2013)</t>
+          <t>(1975)</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
@@ -4983,12 +4983,12 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>To Be or Not to Be</t>
+          <t>The Passion of Joan of Arc</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>(1942)</t>
+          <t>(1928)</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
@@ -5005,12 +5005,12 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Dune</t>
+          <t>Hotel Rwanda</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>(2021)</t>
+          <t>(2004)</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
@@ -5027,12 +5027,12 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>The Big Lebowski</t>
+          <t>Rocky</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>(1998)</t>
+          <t>(1976)</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
@@ -5071,12 +5071,12 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Harry Potter and the Deathly Hallows: Part 2</t>
+          <t>Tokyo Story</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>(2011)</t>
+          <t>(1953)</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
@@ -5093,12 +5093,12 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Ben-Hur</t>
+          <t>Platoon</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>(1959)</t>
+          <t>(1986)</t>
         </is>
       </c>
       <c r="D213" t="inlineStr">
@@ -5115,12 +5115,12 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>How to Train Your Dragon</t>
+          <t>The Terminator</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>(2010)</t>
+          <t>(1984)</t>
         </is>
       </c>
       <c r="D214" t="inlineStr">
@@ -5137,12 +5137,12 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Mad Max: Fury Road</t>
+          <t>Ford v Ferrari</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>(2015)</t>
+          <t>(2019)</t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
@@ -5159,12 +5159,12 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Million Dollar Baby</t>
+          <t>Stand by Me</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>(2004)</t>
+          <t>(1986)</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
@@ -5181,17 +5181,17 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Autumn Sonata</t>
+          <t>Rush</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>(1978)</t>
+          <t>(2013)</t>
         </is>
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>8.0</t>
         </is>
       </c>
     </row>
@@ -5203,17 +5203,17 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>The Wages of Fear</t>
+          <t>Into the Wild</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>(1953)</t>
+          <t>(2007)</t>
         </is>
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>8.0</t>
         </is>
       </c>
     </row>
@@ -5225,17 +5225,17 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Stand by Me</t>
+          <t>The Wizard of Oz</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>(1986)</t>
+          <t>(1939)</t>
         </is>
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>8.0</t>
         </is>
       </c>
     </row>
@@ -5257,7 +5257,7 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>8.0</t>
         </is>
       </c>
     </row>
@@ -5269,17 +5269,17 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Network</t>
+          <t>Spotlight</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>(1976)</t>
+          <t>(2015)</t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>8.0</t>
         </is>
       </c>
     </row>
@@ -5291,17 +5291,17 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>The Handmaiden</t>
+          <t>Network</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>(2016)</t>
+          <t>(1976)</t>
         </is>
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>8.0</t>
         </is>
       </c>
     </row>
@@ -5313,17 +5313,17 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Gangs of Wasseypur</t>
+          <t>Groundhog Day</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>(2012)</t>
+          <t>(1993)</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>8.0</t>
         </is>
       </c>
     </row>
@@ -5335,17 +5335,17 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>La Haine</t>
+          <t>The Exorcist</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>(1995)</t>
+          <t>(1973)</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>8.0</t>
         </is>
       </c>
     </row>
@@ -5357,17 +5357,17 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>A Silent Voice: The Movie</t>
+          <t>Ratatouille</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>(2016)</t>
+          <t>(2007)</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>8.0</t>
         </is>
       </c>
     </row>
@@ -5401,12 +5401,12 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Cool Hand Luke</t>
+          <t>The Incredibles</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>(1967)</t>
+          <t>(2004)</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
@@ -5423,12 +5423,12 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>The 400 Blows</t>
+          <t>Dersu Uzala</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>(1959)</t>
+          <t>(1975)</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
@@ -5445,12 +5445,12 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Platoon</t>
+          <t>The Best Years of Our Lives</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>(1986)</t>
+          <t>(1946)</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
@@ -5467,12 +5467,12 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Spotlight</t>
+          <t>Before Sunset</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>(2015)</t>
+          <t>(2004)</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
@@ -5489,12 +5489,12 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Monsters, Inc.</t>
+          <t>Dune</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>(2001)</t>
+          <t>(2021)</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
@@ -5533,12 +5533,12 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Life of Brian</t>
+          <t>My Father and My Son</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>(1979)</t>
+          <t>(2005)</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
@@ -5555,12 +5555,12 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>In the Mood for Love</t>
+          <t>The Grapes of Wrath</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>(2000)</t>
+          <t>(1940)</t>
         </is>
       </c>
       <c r="D234" t="inlineStr">
@@ -5577,12 +5577,12 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>The Bandit</t>
+          <t>Cool Hand Luke</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>(1996)</t>
+          <t>(1967)</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
@@ -5599,12 +5599,12 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Hotel Rwanda</t>
+          <t>To Be or Not to Be</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>(2004)</t>
+          <t>(1942)</t>
         </is>
       </c>
       <c r="D236" t="inlineStr">
@@ -5621,12 +5621,12 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Rush</t>
+          <t>The Battle of Algiers</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>(2013)</t>
+          <t>(1966)</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
@@ -5643,12 +5643,12 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Rocky</t>
+          <t>Amores perros</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>(1976)</t>
+          <t>(2000)</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
@@ -5665,12 +5665,12 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Demon Slayer the Movie: Mugen Train</t>
+          <t>Pirates of the Caribbean: The Curse of the Black Pearl</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>(2020)</t>
+          <t>(2003)</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
@@ -5687,12 +5687,12 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Amores perros</t>
+          <t>The Sound of Music</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>(2000)</t>
+          <t>(1965)</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
@@ -5709,12 +5709,12 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Into the Wild</t>
+          <t>Life of Brian</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>(2007)</t>
+          <t>(1979)</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
@@ -5731,12 +5731,12 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Nausicaä of the Valley of the Wind</t>
+          <t>The 400 Blows</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>(1984)</t>
+          <t>(1959)</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
@@ -5753,12 +5753,12 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Before Sunset</t>
+          <t>Persona</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>(2004)</t>
+          <t>(1966)</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
@@ -5775,12 +5775,12 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Drishyam</t>
+          <t>It Happened One Night</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>(2013)</t>
+          <t>(1934)</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
@@ -5797,12 +5797,12 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>It Happened One Night</t>
+          <t>La Haine</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>(1934)</t>
+          <t>(1995)</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
@@ -5819,12 +5819,12 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Andrei Rublev</t>
+          <t>Aladdin</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>(1966)</t>
+          <t>(1992)</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
@@ -5841,12 +5841,12 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Miracle in Cell No. 7</t>
+          <t>Jai Bhim</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>(2019)</t>
+          <t>(2021)</t>
         </is>
       </c>
       <c r="D247" t="inlineStr">
@@ -5863,12 +5863,12 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>Beauty and the Beast</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>(2018)</t>
+          <t>(1991)</t>
         </is>
       </c>
       <c r="D248" t="inlineStr">
@@ -5885,7 +5885,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Fanny and Alexander</t>
+          <t>Gandhi</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
@@ -5907,12 +5907,12 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Hera Pheri</t>
+          <t>The Help</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>(2000)</t>
+          <t>(2011)</t>
         </is>
       </c>
       <c r="D250" t="inlineStr">
@@ -5929,12 +5929,12 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Soorarai Pottru</t>
+          <t>The Handmaiden</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>(2020)</t>
+          <t>(2016)</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">

</xml_diff>